<commit_message>
New version of bestelformulier
</commit_message>
<xml_diff>
--- a/static/bestelformulier.xlsx
+++ b/static/bestelformulier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervanes/Documents/Lions/Wijnactie 2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowanvh/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8B5986-C653-634B-B27F-ADF4B0C7D8A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0F4C97-6A29-714A-BD2D-CA2A3EA2CA93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="460" windowWidth="40960" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" r:id="rId1"/>
@@ -20,18 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad2!$C$11:$C$51</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Blad2!$A$1:$I$55</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -229,12 +218,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ [$€-413]\ * #,##0.00_ ;_ [$€-413]\ * \-#,##0.00_ ;_ [$€-413]\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="[$-813]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="_ [$€-413]\ * #,##0.00_ ;_ [$€-413]\ * \-#,##0.00_ ;_ [$€-413]\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="[$-813]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -645,8 +634,8 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="92">
@@ -657,7 +646,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -674,10 +663,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -696,13 +685,13 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -711,7 +700,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -723,7 +712,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -732,7 +721,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -748,7 +737,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -776,7 +765,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -824,19 +813,19 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -860,7 +849,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -887,21 +876,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Goed" xfId="3" builtinId="26"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuta" xfId="2" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -974,7 +963,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1300,7 +1289,7 @@
   <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1620,161 +1609,161 @@
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="13" t="s">
+      <c r="A15" s="60"/>
+      <c r="B15" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="14">
-        <v>7.95</v>
-      </c>
-      <c r="E15" s="15">
-        <f>6*D15</f>
-        <v>47.7</v>
-      </c>
-      <c r="F15" s="49"/>
+      <c r="D15" s="22">
+        <v>7.5</v>
+      </c>
+      <c r="E15" s="22">
+        <f>+D15*6</f>
+        <v>45</v>
+      </c>
+      <c r="F15" s="65"/>
       <c r="G15" s="46"/>
-      <c r="H15" s="50">
-        <f t="shared" ref="H15" si="1">+E15*F15</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="30"/>
+      <c r="H15" s="66">
+        <f>+E15*F15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="61"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="77"/>
+      <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="60"/>
-      <c r="B16" s="72" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="14">
         <v>7.5</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="14">
         <f>+D16*6</f>
         <v>45</v>
       </c>
-      <c r="F16" s="65"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="66">
+      <c r="F16" s="49"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="50">
         <f>+E16*F16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="61"/>
+      <c r="I16" s="30"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="73" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="14">
+    <row r="17" spans="1:14" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="25"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="14">
         <v>7.5</v>
       </c>
-      <c r="E17" s="14">
-        <f>+D17*6</f>
+      <c r="E18" s="14">
+        <f>+D18*6</f>
         <v>45</v>
       </c>
-      <c r="F17" s="49"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="50">
-        <f>+E17*F17</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="30"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="1:14" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="35"/>
-    </row>
-    <row r="19" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="14">
-        <v>7.5</v>
-      </c>
-      <c r="E19" s="14">
-        <f>+D19*6</f>
-        <v>45</v>
-      </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="31">
-        <f>+E19*F19</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="1:14" s="8" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="64"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="35"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="31">
+        <f>+E18*F18</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="36"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="1:14" s="8" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="64"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="14">
+        <v>12.5</v>
+      </c>
+      <c r="E20" s="15">
+        <f>6*D20</f>
+        <v>75</v>
+      </c>
+      <c r="F20" s="49"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="50">
+        <f t="shared" ref="H20:H24" si="1">+E20*F20</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="30"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
     </row>
     <row r="21" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="14">
-        <v>12.5</v>
-      </c>
-      <c r="E21" s="15">
+      <c r="D21" s="24">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E21" s="68">
         <f>6*D21</f>
-        <v>75</v>
-      </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="50">
-        <f t="shared" ref="H21:H24" si="2">+E21*F21</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="30"/>
+        <v>53.699999999999996</v>
+      </c>
+      <c r="F21" s="69"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="62"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -1782,31 +1771,31 @@
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="23" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="24">
-        <v>8.9499999999999993</v>
-      </c>
-      <c r="E22" s="68">
+      <c r="D22" s="14">
+        <v>7.95</v>
+      </c>
+      <c r="E22" s="15">
         <f>6*D22</f>
-        <v>53.699999999999996</v>
-      </c>
-      <c r="F22" s="69"/>
+        <v>47.7</v>
+      </c>
+      <c r="F22" s="49"/>
       <c r="G22" s="46"/>
-      <c r="H22" s="70">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="62"/>
+      <c r="H22" s="50">
+        <f>+E22*F22</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="30"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
+      <c r="M22" s="77"/>
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1827,7 +1816,7 @@
       <c r="F23" s="49"/>
       <c r="G23" s="46"/>
       <c r="H23" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I23" s="30"/>
@@ -1855,7 +1844,7 @@
       <c r="F24" s="49"/>
       <c r="G24" s="44"/>
       <c r="H24" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I24" s="30"/>
@@ -1916,15 +1905,15 @@
         <v>0</v>
       </c>
       <c r="G27" s="5">
-        <f t="shared" ref="G27:I27" si="3">SUM(G11:G24)</f>
+        <f>SUM(G11:G24)</f>
         <v>0</v>
       </c>
       <c r="H27" s="80">
-        <f t="shared" si="3"/>
+        <f>SUM(H11:H24)</f>
         <v>0</v>
       </c>
       <c r="I27" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(I11:I24)</f>
         <v>0</v>
       </c>
       <c r="J27" s="7"/>
@@ -2184,13 +2173,13 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="E37" s="15">
-        <f t="shared" ref="E37" si="4">6*D37</f>
+        <f t="shared" ref="E37" si="2">6*D37</f>
         <v>53.699999999999996</v>
       </c>
       <c r="F37" s="42"/>
       <c r="G37" s="44"/>
       <c r="H37" s="31">
-        <f t="shared" ref="H37" si="5">+E37*F37</f>
+        <f t="shared" ref="H37" si="3">+E37*F37</f>
         <v>0</v>
       </c>
       <c r="I37" s="30"/>
@@ -2251,13 +2240,13 @@
         <v>15.4</v>
       </c>
       <c r="E40" s="15">
-        <f t="shared" ref="E40" si="6">6*D40</f>
+        <f t="shared" ref="E40" si="4">6*D40</f>
         <v>92.4</v>
       </c>
       <c r="F40" s="49"/>
       <c r="G40" s="43"/>
       <c r="H40" s="50">
-        <f t="shared" ref="H40" si="7">+E40*F40</f>
+        <f t="shared" ref="H40" si="5">+E40*F40</f>
         <v>0</v>
       </c>
       <c r="I40" s="30"/>
@@ -2311,13 +2300,13 @@
         <v>11.95</v>
       </c>
       <c r="E42" s="15">
-        <f t="shared" ref="E42" si="8">6*D42</f>
+        <f t="shared" ref="E42" si="6">6*D42</f>
         <v>71.699999999999989</v>
       </c>
       <c r="F42" s="49"/>
       <c r="G42" s="46"/>
       <c r="H42" s="50">
-        <f t="shared" ref="H42" si="9">+E42*F42</f>
+        <f t="shared" ref="H42" si="7">+E42*F42</f>
         <v>0</v>
       </c>
       <c r="I42" s="30"/>
@@ -2431,13 +2420,13 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="E46" s="15">
-        <f t="shared" ref="E46:E47" si="10">6*D46</f>
+        <f t="shared" ref="E46:E47" si="8">6*D46</f>
         <v>53.699999999999996</v>
       </c>
       <c r="F46" s="49"/>
       <c r="G46" s="46"/>
       <c r="H46" s="50">
-        <f t="shared" ref="H46:H47" si="11">+E46*F46</f>
+        <f t="shared" ref="H46:H47" si="9">+E46*F46</f>
         <v>0</v>
       </c>
       <c r="I46" s="30"/>
@@ -2461,13 +2450,13 @@
         <v>8.75</v>
       </c>
       <c r="E47" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>52.5</v>
       </c>
       <c r="F47" s="49"/>
       <c r="G47" s="44"/>
       <c r="H47" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I47" s="30"/>
@@ -2616,15 +2605,15 @@
         <v>0</v>
       </c>
       <c r="G54" s="5">
-        <f t="shared" ref="G54:I54" si="12">SUM(G31:G51)</f>
+        <f t="shared" ref="G54:I54" si="10">SUM(G31:G51)</f>
         <v>0</v>
       </c>
       <c r="H54" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I54" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J54" s="7"/>
@@ -2684,15 +2673,15 @@
         <v>0</v>
       </c>
       <c r="G57" s="5">
-        <f t="shared" ref="G57:I57" si="13">G54+G27</f>
+        <f t="shared" ref="G57:I57" si="11">G54+G27</f>
         <v>0</v>
       </c>
       <c r="H57" s="80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I57" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J57" s="7"/>

</xml_diff>